<commit_message>
Lab 8 finishing touches
</commit_message>
<xml_diff>
--- a/testfiles/ExpectedResultsTable.xlsx
+++ b/testfiles/ExpectedResultsTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\ELC3338\Team9\ARM-Lab_Spring2019_S1_P2_Team9\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D497B3-D26D-4D81-927C-9D21A4DD0427}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296E986D-BA0F-4EC6-9B8F-96209D27E814}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="68">
   <si>
     <t>Instruction 1</t>
   </si>
@@ -606,7 +606,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,35 +1216,35 @@
       <c r="A18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="10">
-        <v>4</v>
-      </c>
-      <c r="C18" s="10">
-        <v>8</v>
-      </c>
-      <c r="D18" s="10">
-        <v>12</v>
-      </c>
-      <c r="E18" s="10">
-        <v>16</v>
+      <c r="B18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="F18" s="10">
-        <v>20</v>
+        <v>-20</v>
       </c>
       <c r="G18" s="10">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="H18" s="10">
         <v>28</v>
       </c>
       <c r="I18" s="10">
-        <v>32</v>
+        <v>256</v>
       </c>
       <c r="J18" s="10">
-        <v>36</v>
-      </c>
-      <c r="K18" s="10">
-        <v>40</v>
+        <v>-220</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>